<commit_message>
Actualización de archivos JSON y scripts 06 de enero 2026
</commit_message>
<xml_diff>
--- a/Tuya.xlsx
+++ b/Tuya.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="508" uniqueCount="259">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="528" uniqueCount="267">
   <si>
     <t>Asignado a</t>
   </si>
@@ -885,6 +885,30 @@
   </si>
   <si>
     <t>31/12/2025: Se realiza la validación con el area encargada y se brinda colaboración para volver a inciar el servicio el cual quedo inactivo luego de un reinicio</t>
+  </si>
+  <si>
+    <t>329</t>
+  </si>
+  <si>
+    <t>330</t>
+  </si>
+  <si>
+    <t>Soporte Imagine</t>
+  </si>
+  <si>
+    <t>Solicitaron revision de reporte de imagenes eliminadas ya que no encuentran las imagenes</t>
+  </si>
+  <si>
+    <t>05/01/2026: Se realizan las validaciones sobre las solicitudes reprotadas, se hace un analisis de los los y se brinda la información sobre el proceso para las imagenes eliminadas y como funciona la revisión de los logs.</t>
+  </si>
+  <si>
+    <t>331</t>
+  </si>
+  <si>
+    <t>Ajuste Log API Imagine</t>
+  </si>
+  <si>
+    <t>Se recibe requerimiento en el cual se solicita ajustar los logs del API de Imagine para que guarde el body que se esta enviando en las peticiones que fallan al entregar documentos al servicio del cliente</t>
   </si>
   <si>
     <t xml:space="preserve"> Año Nuevo</t>
@@ -1918,22 +1942,7 @@
     <xf borderId="5" fillId="3" fontId="14" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" readingOrder="0" vertical="center"/>
     </xf>
-    <xf borderId="5" fillId="4" fontId="32" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf borderId="5" fillId="4" fontId="14" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf borderId="5" fillId="4" fontId="35" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf borderId="5" fillId="4" fontId="9" numFmtId="3" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf borderId="5" fillId="4" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf borderId="5" fillId="4" fontId="9" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf borderId="5" fillId="3" fontId="32" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
@@ -1955,6 +1964,21 @@
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf borderId="5" fillId="3" fontId="9" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf borderId="5" fillId="4" fontId="32" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf borderId="5" fillId="4" fontId="14" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf borderId="5" fillId="4" fontId="35" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf borderId="5" fillId="4" fontId="9" numFmtId="3" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf borderId="5" fillId="4" fontId="9" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf borderId="12" fillId="3" fontId="32" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
@@ -2478,7 +2502,7 @@
       <c r="L2" s="22"/>
       <c r="M2" s="23">
         <f>IF(ISBLANK(L2), NETWORKDAYS(J2, TODAY(),Hoja2!$A$1:$A$18), NETWORKDAYS(J2, L2, Hoja2!$A$1:$A$18))</f>
-        <v>254</v>
+        <v>258</v>
       </c>
       <c r="N2" s="24"/>
       <c r="O2" s="25"/>
@@ -2540,7 +2564,7 @@
       <c r="L3" s="37"/>
       <c r="M3" s="38">
         <f>IF(ISBLANK(L3), NETWORKDAYS(J3, TODAY(),Hoja2!$A$1:$A$18), NETWORKDAYS(J3, L3, Hoja2!$A$1:$A$18))</f>
-        <v>254</v>
+        <v>258</v>
       </c>
       <c r="N3" s="39"/>
       <c r="O3" s="40"/>
@@ -2602,7 +2626,7 @@
       <c r="L4" s="22"/>
       <c r="M4" s="23">
         <f>IF(ISBLANK(L4), NETWORKDAYS(J4, TODAY(),Hoja2!$A$1:$A$18), NETWORKDAYS(J4, L4, Hoja2!$A$1:$A$18))</f>
-        <v>254</v>
+        <v>258</v>
       </c>
       <c r="N4" s="22"/>
       <c r="O4" s="25"/>
@@ -2664,7 +2688,7 @@
       <c r="L5" s="36"/>
       <c r="M5" s="38">
         <f>IF(ISBLANK(L5), NETWORKDAYS(J5, TODAY(),Hoja2!$A$1:$A$18), NETWORKDAYS(J5, L5, Hoja2!$A$1:$A$18))</f>
-        <v>254</v>
+        <v>258</v>
       </c>
       <c r="N5" s="39"/>
       <c r="O5" s="40"/>
@@ -2726,7 +2750,7 @@
       <c r="L6" s="22"/>
       <c r="M6" s="23">
         <f>IF(ISBLANK(L6), NETWORKDAYS(J6, TODAY(),Hoja2!$A$1:$A$18), NETWORKDAYS(J6, L6, Hoja2!$A$1:$A$18))</f>
-        <v>254</v>
+        <v>258</v>
       </c>
       <c r="N6" s="24"/>
       <c r="O6" s="25"/>
@@ -2788,7 +2812,7 @@
       <c r="L7" s="46"/>
       <c r="M7" s="38">
         <f>IF(ISBLANK(L7), NETWORKDAYS(J7, TODAY(),Hoja2!$A$1:$A$18), NETWORKDAYS(J7, L7, Hoja2!$A$1:$A$18))</f>
-        <v>254</v>
+        <v>258</v>
       </c>
       <c r="N7" s="47"/>
       <c r="O7" s="48"/>
@@ -2850,7 +2874,7 @@
       <c r="L8" s="22"/>
       <c r="M8" s="23">
         <f>IF(ISBLANK(L8), NETWORKDAYS(J8, TODAY(),Hoja2!$A$1:$A$18), NETWORKDAYS(J8, L8, Hoja2!$A$1:$A$18))</f>
-        <v>254</v>
+        <v>258</v>
       </c>
       <c r="N8" s="22"/>
       <c r="O8" s="52"/>
@@ -2912,7 +2936,7 @@
       <c r="L9" s="36"/>
       <c r="M9" s="38">
         <f>IF(ISBLANK(L9), NETWORKDAYS(J9, TODAY(),Hoja2!$A$1:$A$18), NETWORKDAYS(J9, L9, Hoja2!$A$1:$A$18))</f>
-        <v>137</v>
+        <v>141</v>
       </c>
       <c r="N9" s="47"/>
       <c r="O9" s="48"/>
@@ -2974,7 +2998,7 @@
       <c r="L10" s="22"/>
       <c r="M10" s="23">
         <f>IF(ISBLANK(L10), NETWORKDAYS(J10, TODAY(),Hoja2!$A$1:$A$18), NETWORKDAYS(J10, L10, Hoja2!$A$1:$A$18))</f>
-        <v>137</v>
+        <v>141</v>
       </c>
       <c r="N10" s="22"/>
       <c r="O10" s="52"/>
@@ -3034,7 +3058,7 @@
       <c r="L11" s="37"/>
       <c r="M11" s="38">
         <f>IF(ISBLANK(L11), NETWORKDAYS(J11, TODAY(),Hoja2!$A$1:$A$18), NETWORKDAYS(J11, L11, Hoja2!$A$1:$A$18))</f>
-        <v>137</v>
+        <v>141</v>
       </c>
       <c r="N11" s="37"/>
       <c r="O11" s="48"/>
@@ -3096,7 +3120,7 @@
       <c r="L12" s="22"/>
       <c r="M12" s="23">
         <f>IF(ISBLANK(L12), NETWORKDAYS(J12, TODAY(),Hoja2!$A$1:$A$18), NETWORKDAYS(J12, L12, Hoja2!$A$1:$A$18))</f>
-        <v>137</v>
+        <v>141</v>
       </c>
       <c r="N12" s="22"/>
       <c r="O12" s="52"/>
@@ -3156,7 +3180,7 @@
       <c r="L13" s="37"/>
       <c r="M13" s="38">
         <f>IF(ISBLANK(L13), NETWORKDAYS(J13, TODAY(),Hoja2!$A$1:$A$18), NETWORKDAYS(J13, L13, Hoja2!$A$1:$A$18))</f>
-        <v>32857</v>
+        <v>32861</v>
       </c>
       <c r="N13" s="37"/>
       <c r="O13" s="48"/>
@@ -3220,7 +3244,7 @@
       <c r="L14" s="22"/>
       <c r="M14" s="23">
         <f>IF(ISBLANK(L14), NETWORKDAYS(J14, TODAY(),Hoja2!$A$1:$A$18), NETWORKDAYS(J14, L14, Hoja2!$A$1:$A$18))</f>
-        <v>140</v>
+        <v>144</v>
       </c>
       <c r="N14" s="22"/>
       <c r="O14" s="52"/>
@@ -3284,7 +3308,7 @@
       <c r="L15" s="37"/>
       <c r="M15" s="38">
         <f>IF(ISBLANK(L15), NETWORKDAYS(J15, TODAY(),Hoja2!$A$1:$A$18), NETWORKDAYS(J15, L15, Hoja2!$A$1:$A$18))</f>
-        <v>140</v>
+        <v>144</v>
       </c>
       <c r="N15" s="37"/>
       <c r="O15" s="48"/>
@@ -3414,7 +3438,7 @@
       <c r="L17" s="37"/>
       <c r="M17" s="38">
         <f>IF(ISBLANK(L17), NETWORKDAYS(J17, TODAY(),Hoja2!$A$1:$A$18), NETWORKDAYS(J17, L17, Hoja2!$A$1:$A$18))</f>
-        <v>139</v>
+        <v>143</v>
       </c>
       <c r="N17" s="37"/>
       <c r="O17" s="48"/>
@@ -3616,7 +3640,7 @@
       <c r="L20" s="88"/>
       <c r="M20" s="23">
         <f>IF(ISBLANK(L20), NETWORKDAYS(J20, TODAY(),Hoja2!$A$1:$A$18), NETWORKDAYS(J20, L20, Hoja2!$A$1:$A$18))</f>
-        <v>136</v>
+        <v>140</v>
       </c>
       <c r="N20" s="96"/>
       <c r="O20" s="52"/>
@@ -4562,7 +4586,7 @@
       <c r="L35" s="46"/>
       <c r="M35" s="38">
         <f>IF(ISBLANK(L35), NETWORKDAYS(J35, TODAY(),Hoja2!$A$1:$A$18), NETWORKDAYS(J35, L35, Hoja2!$A$1:$A$18))</f>
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="N35" s="92">
         <v>45953.0</v>
@@ -5076,7 +5100,7 @@
       <c r="L43" s="90"/>
       <c r="M43" s="38">
         <f>IF(ISBLANK(L43), NETWORKDAYS(J43, TODAY(),Hoja2!$A$1:$A$18), NETWORKDAYS(J43, L43, Hoja2!$A$1:$A$18))</f>
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="N43" s="47"/>
       <c r="O43" s="48"/>
@@ -6862,23 +6886,46 @@
       <c r="AM70" s="132"/>
     </row>
     <row r="71">
-      <c r="A71" s="167"/>
-      <c r="B71" s="168"/>
-      <c r="C71" s="169"/>
-      <c r="D71" s="114"/>
+      <c r="A71" s="29" t="s">
+        <v>23</v>
+      </c>
+      <c r="B71" s="30" t="s">
+        <v>241</v>
+      </c>
+      <c r="C71" s="102" t="s">
+        <v>202</v>
+      </c>
+      <c r="D71" s="108" t="s">
+        <v>209</v>
+      </c>
       <c r="E71" s="114"/>
-      <c r="F71" s="45"/>
-      <c r="G71" s="170"/>
+      <c r="F71" s="124" t="s">
+        <v>36</v>
+      </c>
+      <c r="G71" s="125">
+        <v>100.0</v>
+      </c>
       <c r="H71" s="115"/>
       <c r="I71" s="47"/>
-      <c r="J71" s="46"/>
+      <c r="J71" s="116">
+        <v>45662.0</v>
+      </c>
       <c r="K71" s="46"/>
-      <c r="L71" s="46"/>
-      <c r="M71" s="64"/>
+      <c r="L71" s="116">
+        <v>45662.0</v>
+      </c>
+      <c r="M71" s="151">
+        <f>IF(ISBLANK(L71), NETWORKDAYS(J71, TODAY(),Hoja2!$A$1:$A$18), NETWORKDAYS(J71, L71, Hoja2!$A$1:$A$18))</f>
+        <v>0</v>
+      </c>
       <c r="N71" s="47"/>
       <c r="O71" s="48"/>
-      <c r="P71" s="171"/>
-      <c r="Q71" s="172"/>
+      <c r="P71" s="120" t="s">
+        <v>203</v>
+      </c>
+      <c r="Q71" s="42" t="s">
+        <v>16</v>
+      </c>
       <c r="R71" s="134"/>
       <c r="S71" s="135"/>
       <c r="T71" s="135"/>
@@ -6903,23 +6950,43 @@
       <c r="AM71" s="136"/>
     </row>
     <row r="72">
-      <c r="A72" s="173"/>
-      <c r="B72" s="174"/>
-      <c r="C72" s="175"/>
-      <c r="D72" s="111"/>
+      <c r="A72" s="137" t="s">
+        <v>17</v>
+      </c>
+      <c r="B72" s="166" t="s">
+        <v>242</v>
+      </c>
+      <c r="C72" s="158" t="s">
+        <v>243</v>
+      </c>
+      <c r="D72" s="109" t="s">
+        <v>244</v>
+      </c>
       <c r="E72" s="111"/>
-      <c r="F72" s="176"/>
-      <c r="G72" s="177"/>
+      <c r="F72" s="126" t="s">
+        <v>36</v>
+      </c>
+      <c r="G72" s="127">
+        <v>100.0</v>
+      </c>
       <c r="H72" s="112"/>
       <c r="I72" s="96"/>
-      <c r="J72" s="88"/>
+      <c r="J72" s="77">
+        <v>46027.0</v>
+      </c>
       <c r="K72" s="88"/>
-      <c r="L72" s="88"/>
+      <c r="L72" s="77">
+        <v>46034.0</v>
+      </c>
       <c r="M72" s="68"/>
       <c r="N72" s="96"/>
       <c r="O72" s="52"/>
-      <c r="P72" s="178"/>
-      <c r="Q72" s="179"/>
+      <c r="P72" s="160" t="s">
+        <v>245</v>
+      </c>
+      <c r="Q72" s="161" t="s">
+        <v>16</v>
+      </c>
       <c r="R72" s="138"/>
       <c r="S72" s="131"/>
       <c r="T72" s="131"/>
@@ -6944,13 +7011,25 @@
       <c r="AM72" s="132"/>
     </row>
     <row r="73">
-      <c r="A73" s="167"/>
-      <c r="B73" s="168"/>
-      <c r="C73" s="169"/>
-      <c r="D73" s="114"/>
+      <c r="A73" s="133" t="s">
+        <v>17</v>
+      </c>
+      <c r="B73" s="162" t="s">
+        <v>246</v>
+      </c>
+      <c r="C73" s="163" t="s">
+        <v>247</v>
+      </c>
+      <c r="D73" s="108" t="s">
+        <v>248</v>
+      </c>
       <c r="E73" s="114"/>
-      <c r="F73" s="45"/>
-      <c r="G73" s="170"/>
+      <c r="F73" s="124" t="s">
+        <v>159</v>
+      </c>
+      <c r="G73" s="125">
+        <v>0.0</v>
+      </c>
       <c r="H73" s="115"/>
       <c r="I73" s="47"/>
       <c r="J73" s="46"/>
@@ -6959,8 +7038,10 @@
       <c r="M73" s="64"/>
       <c r="N73" s="47"/>
       <c r="O73" s="48"/>
-      <c r="P73" s="171"/>
-      <c r="Q73" s="172"/>
+      <c r="P73" s="167"/>
+      <c r="Q73" s="165" t="s">
+        <v>16</v>
+      </c>
       <c r="R73" s="134"/>
       <c r="S73" s="135"/>
       <c r="T73" s="135"/>
@@ -6985,13 +7066,13 @@
       <c r="AM73" s="136"/>
     </row>
     <row r="74">
-      <c r="A74" s="173"/>
-      <c r="B74" s="174"/>
-      <c r="C74" s="175"/>
+      <c r="A74" s="168"/>
+      <c r="B74" s="169"/>
+      <c r="C74" s="170"/>
       <c r="D74" s="111"/>
       <c r="E74" s="111"/>
-      <c r="F74" s="176"/>
-      <c r="G74" s="177"/>
+      <c r="F74" s="171"/>
+      <c r="G74" s="172"/>
       <c r="H74" s="112"/>
       <c r="I74" s="96"/>
       <c r="J74" s="88"/>
@@ -7000,8 +7081,8 @@
       <c r="M74" s="68"/>
       <c r="N74" s="96"/>
       <c r="O74" s="52"/>
-      <c r="P74" s="178"/>
-      <c r="Q74" s="179"/>
+      <c r="P74" s="173"/>
+      <c r="Q74" s="174"/>
       <c r="R74" s="138"/>
       <c r="S74" s="131"/>
       <c r="T74" s="131"/>
@@ -7026,13 +7107,13 @@
       <c r="AM74" s="132"/>
     </row>
     <row r="75">
-      <c r="A75" s="167"/>
-      <c r="B75" s="168"/>
-      <c r="C75" s="169"/>
+      <c r="A75" s="175"/>
+      <c r="B75" s="176"/>
+      <c r="C75" s="177"/>
       <c r="D75" s="114"/>
       <c r="E75" s="114"/>
       <c r="F75" s="45"/>
-      <c r="G75" s="170"/>
+      <c r="G75" s="178"/>
       <c r="H75" s="115"/>
       <c r="I75" s="47"/>
       <c r="J75" s="46"/>
@@ -7041,8 +7122,8 @@
       <c r="M75" s="64"/>
       <c r="N75" s="47"/>
       <c r="O75" s="48"/>
-      <c r="P75" s="171"/>
-      <c r="Q75" s="172"/>
+      <c r="P75" s="167"/>
+      <c r="Q75" s="179"/>
       <c r="R75" s="134"/>
       <c r="S75" s="135"/>
       <c r="T75" s="135"/>
@@ -7067,13 +7148,13 @@
       <c r="AM75" s="136"/>
     </row>
     <row r="76">
-      <c r="A76" s="173"/>
-      <c r="B76" s="174"/>
-      <c r="C76" s="175"/>
+      <c r="A76" s="168"/>
+      <c r="B76" s="169"/>
+      <c r="C76" s="170"/>
       <c r="D76" s="111"/>
       <c r="E76" s="111"/>
-      <c r="F76" s="176"/>
-      <c r="G76" s="177"/>
+      <c r="F76" s="171"/>
+      <c r="G76" s="172"/>
       <c r="H76" s="112"/>
       <c r="I76" s="96"/>
       <c r="J76" s="88"/>
@@ -7082,8 +7163,8 @@
       <c r="M76" s="68"/>
       <c r="N76" s="96"/>
       <c r="O76" s="52"/>
-      <c r="P76" s="178"/>
-      <c r="Q76" s="179"/>
+      <c r="P76" s="173"/>
+      <c r="Q76" s="174"/>
       <c r="R76" s="138"/>
       <c r="S76" s="131"/>
       <c r="T76" s="131"/>
@@ -7108,13 +7189,13 @@
       <c r="AM76" s="132"/>
     </row>
     <row r="77">
-      <c r="A77" s="167"/>
-      <c r="B77" s="168"/>
-      <c r="C77" s="169"/>
+      <c r="A77" s="175"/>
+      <c r="B77" s="176"/>
+      <c r="C77" s="177"/>
       <c r="D77" s="114"/>
       <c r="E77" s="114"/>
       <c r="F77" s="45"/>
-      <c r="G77" s="170"/>
+      <c r="G77" s="178"/>
       <c r="H77" s="115"/>
       <c r="I77" s="47"/>
       <c r="J77" s="46"/>
@@ -7123,8 +7204,8 @@
       <c r="M77" s="64"/>
       <c r="N77" s="47"/>
       <c r="O77" s="48"/>
-      <c r="P77" s="171"/>
-      <c r="Q77" s="172"/>
+      <c r="P77" s="167"/>
+      <c r="Q77" s="179"/>
       <c r="R77" s="134"/>
       <c r="S77" s="135"/>
       <c r="T77" s="135"/>
@@ -42858,7 +42939,7 @@
         <v>45292.0</v>
       </c>
       <c r="B1" s="232" t="s">
-        <v>241</v>
+        <v>249</v>
       </c>
     </row>
     <row r="2" ht="17.25" customHeight="1">
@@ -42866,7 +42947,7 @@
         <v>45299.0</v>
       </c>
       <c r="B2" s="232" t="s">
-        <v>242</v>
+        <v>250</v>
       </c>
     </row>
     <row r="3" ht="17.25" customHeight="1">
@@ -42874,7 +42955,7 @@
         <v>45376.0</v>
       </c>
       <c r="B3" s="232" t="s">
-        <v>243</v>
+        <v>251</v>
       </c>
     </row>
     <row r="4" ht="17.25" customHeight="1">
@@ -42882,7 +42963,7 @@
         <v>45379.0</v>
       </c>
       <c r="B4" s="232" t="s">
-        <v>244</v>
+        <v>252</v>
       </c>
     </row>
     <row r="5" ht="17.25" customHeight="1">
@@ -42890,7 +42971,7 @@
         <v>45380.0</v>
       </c>
       <c r="B5" s="232" t="s">
-        <v>245</v>
+        <v>253</v>
       </c>
     </row>
     <row r="6" ht="17.25" customHeight="1">
@@ -42898,7 +42979,7 @@
         <v>45413.0</v>
       </c>
       <c r="B6" s="232" t="s">
-        <v>246</v>
+        <v>254</v>
       </c>
     </row>
     <row r="7" ht="17.25" customHeight="1">
@@ -42906,7 +42987,7 @@
         <v>45425.0</v>
       </c>
       <c r="B7" s="232" t="s">
-        <v>247</v>
+        <v>255</v>
       </c>
     </row>
     <row r="8" ht="17.25" customHeight="1">
@@ -42914,7 +42995,7 @@
         <v>45446.0</v>
       </c>
       <c r="B8" s="232" t="s">
-        <v>248</v>
+        <v>256</v>
       </c>
     </row>
     <row r="9" ht="17.25" customHeight="1">
@@ -42922,7 +43003,7 @@
         <v>45453.0</v>
       </c>
       <c r="B9" s="232" t="s">
-        <v>249</v>
+        <v>257</v>
       </c>
     </row>
     <row r="10" ht="17.25" customHeight="1">
@@ -42930,7 +43011,7 @@
         <v>45474.0</v>
       </c>
       <c r="B10" s="232" t="s">
-        <v>250</v>
+        <v>258</v>
       </c>
     </row>
     <row r="11" ht="17.25" customHeight="1">
@@ -42938,7 +43019,7 @@
         <v>45493.0</v>
       </c>
       <c r="B11" s="232" t="s">
-        <v>251</v>
+        <v>259</v>
       </c>
     </row>
     <row r="12" ht="17.25" customHeight="1">
@@ -42946,7 +43027,7 @@
         <v>45511.0</v>
       </c>
       <c r="B12" s="232" t="s">
-        <v>252</v>
+        <v>260</v>
       </c>
     </row>
     <row r="13" ht="17.25" customHeight="1">
@@ -42954,7 +43035,7 @@
         <v>45523.0</v>
       </c>
       <c r="B13" s="232" t="s">
-        <v>253</v>
+        <v>261</v>
       </c>
     </row>
     <row r="14" ht="17.25" customHeight="1">
@@ -42962,7 +43043,7 @@
         <v>45579.0</v>
       </c>
       <c r="B14" s="232" t="s">
-        <v>254</v>
+        <v>262</v>
       </c>
     </row>
     <row r="15" ht="17.25" customHeight="1">
@@ -42970,7 +43051,7 @@
         <v>45600.0</v>
       </c>
       <c r="B15" s="232" t="s">
-        <v>255</v>
+        <v>263</v>
       </c>
     </row>
     <row r="16" ht="17.25" customHeight="1">
@@ -42978,7 +43059,7 @@
         <v>45607.0</v>
       </c>
       <c r="B16" s="232" t="s">
-        <v>256</v>
+        <v>264</v>
       </c>
     </row>
     <row r="17" ht="17.25" customHeight="1">
@@ -42986,7 +43067,7 @@
         <v>45634.0</v>
       </c>
       <c r="B17" s="232" t="s">
-        <v>257</v>
+        <v>265</v>
       </c>
     </row>
     <row r="18" ht="17.25" customHeight="1">
@@ -42994,7 +43075,7 @@
         <v>45651.0</v>
       </c>
       <c r="B18" s="232" t="s">
-        <v>258</v>
+        <v>266</v>
       </c>
     </row>
     <row r="19" ht="17.25" customHeight="1"/>

</xml_diff>